<commit_message>
Swapped the NetServices and TrustSec_Devices SGACLs
</commit_message>
<xml_diff>
--- a/ise_trustsec_matrix_thomas.xlsx
+++ b/ise_trustsec_matrix_thomas.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/hack/Projects/Cisco_ISE_Meraki_TrustSec_Scripts/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2B418E-05F1-B94B-8E7A-F4B5B1550FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="38400" yWindow="21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="SGACLs" sheetId="2" r:id="rId2"/>
     <sheet name="SGTs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="41">
   <si>
     <t>SGT</t>
   </si>
@@ -176,8 +182,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,11 +253,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FF64BBE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEF7775"/>
         </patternFill>
       </fill>
     </dxf>
@@ -265,26 +278,41 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEF7775"/>
+          <bgColor rgb="FF6CC04A"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF64BBE3"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -322,7 +350,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -356,6 +384,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -390,9 +419,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -565,20 +595,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
-    <col min="4" max="11" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="11" width="12.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -613,7 +643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -645,7 +675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -677,7 +707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -709,7 +739,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -741,7 +771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -752,16 +782,16 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>15</v>
@@ -770,13 +800,13 @@
         <v>15</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -787,16 +817,16 @@
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>15</v>
@@ -805,13 +835,13 @@
         <v>15</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -846,7 +876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -880,22 +910,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:K9">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="default">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="default">
       <formula>NOT(ISERROR(SEARCH("default",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="allow">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="allow">
       <formula>NOT(ISERROR(SEARCH("allow",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="permit">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="permit">
       <formula>NOT(ISERROR(SEARCH("permit",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="deny">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="deny">
       <formula>NOT(ISERROR(SEARCH("deny",D2)))</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="6">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -904,14 +934,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -928,7 +958,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -942,7 +972,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -956,7 +986,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -970,7 +1000,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -984,7 +1014,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -998,7 +1028,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1012,7 +1042,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1026,7 +1056,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1046,14 +1076,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
@@ -1073,7 +1103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>18</v>
       </c>
@@ -1090,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>18</v>
       </c>
@@ -1107,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>18</v>
       </c>
@@ -1124,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>18</v>
       </c>
@@ -1141,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>18</v>
       </c>
@@ -1161,7 +1191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>18</v>
       </c>
@@ -1181,7 +1211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>18</v>
       </c>
@@ -1201,7 +1231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>18</v>
       </c>
@@ -1218,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>18</v>
       </c>

</xml_diff>